<commit_message>
update on PA Data analysis
</commit_message>
<xml_diff>
--- a/Vale/Docs/DataPA/PA_Summary_2023.xlsx
+++ b/Vale/Docs/DataPA/PA_Summary_2023.xlsx
@@ -25,9 +25,6 @@
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
-    <externalReference r:id="rId18"/>
-    <externalReference r:id="rId19"/>
-    <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
     <definedName function="false" hidden="false" name="aclbseadj" vbProcedure="false">[6]Data!$FL$6:$FL$57</definedName>
@@ -228,13 +225,11 @@
     <definedName function="false" hidden="false" name="factors" vbProcedure="false">[16]PARAMETER!$B$5:$I$12</definedName>
     <definedName function="false" hidden="false" name="FCEPAR" vbProcedure="false">[2]efledger!#ref!</definedName>
     <definedName function="false" hidden="false" name="FEB" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="Feedrate_Cht" vbProcedure="false">'[17]Feed rate_cht'!$B$68:$L$125</definedName>
     <definedName function="false" hidden="false" name="Feed_rate_Cht" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="FE_EFS1" vbProcedure="false">[11]Update_Data!$AE$2:$AH$45</definedName>
     <definedName function="false" hidden="false" name="FLUX" vbProcedure="false">[2]CVLEDGER!$A$1:$L$16</definedName>
     <definedName function="false" hidden="false" name="Flux_Blended" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="FOR_MACRO" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="free" vbProcedure="false">[18]assumptions!#ref!</definedName>
     <definedName function="false" hidden="false" name="GRAPH_ACT" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="GRA_BASE" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="GRA_BASE_MIN" vbProcedure="false">#REF!</definedName>
@@ -273,7 +268,6 @@
     <definedName function="false" hidden="false" name="MAY" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Mech_Av" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Metal_Balance" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="MP_Inv" vbProcedure="false">[19]MP_Inv!$A$2:$A$54</definedName>
     <definedName function="false" hidden="false" name="Mtce_Av" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="mth" vbProcedure="false">[6]Data!$C$6:$C$57</definedName>
     <definedName function="false" hidden="false" name="NOV" vbProcedure="false">#REF!</definedName>
@@ -291,7 +285,6 @@
     <definedName function="false" hidden="false" name="OB_rate5130FS" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="OCT" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="ONHAND" vbProcedure="false">[2]CVLEDGER!$A$194:$I$210</definedName>
-    <definedName function="false" hidden="false" name="Opt_Cht" vbProcedure="false">[17]availability!#ref!</definedName>
     <definedName function="false" hidden="false" name="PA" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Page1" vbProcedure="false">[5]PRODUCTION!$A$1:$G$52</definedName>
     <definedName function="false" hidden="false" name="Page1MR" vbProcedure="false">[5]PRODUCTION!$A$1:$G$68</definedName>
@@ -402,13 +395,11 @@
     <definedName function="false" hidden="false" name="Scr._Sta_reject" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="SCRAP" vbProcedure="false">[2]CVLEDGER!$A$18:$L$64</definedName>
     <definedName function="false" hidden="false" name="SCRAPRK" vbProcedure="false">[2]rkledger!#ref!</definedName>
-    <definedName function="false" hidden="false" name="SCrap_inv" vbProcedure="false">[19]Scrap_Inv!$A$1:$F$49</definedName>
     <definedName function="false" hidden="false" name="SEP" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="SG_Slag" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Shiftly_Cht" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Shift_Data" vbProcedure="false">'[13]52 wks rolling data'!$B$60:$G$102</definedName>
     <definedName function="false" hidden="false" name="Shift_Data_EF" vbProcedure="false">'[13]52 wks rolling data'!#ref!</definedName>
-    <definedName function="false" hidden="false" name="shift_tgl" vbProcedure="false">[20]shift!$C$20:$C$1174</definedName>
     <definedName function="false" hidden="false" name="SHIP" vbProcedure="false">[2]CVLEDGER!$A$177:$I$192</definedName>
     <definedName function="false" hidden="false" name="SM_ADJ" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Sp1A" vbProcedure="false">#REF!</definedName>
@@ -1486,7 +1477,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="129">
   <si>
     <t xml:space="preserve">Unit</t>
   </si>
@@ -1755,7 +1746,19 @@
     <t xml:space="preserve">Remarks</t>
   </si>
   <si>
-    <t xml:space="preserve">Event Time</t>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGS Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity or Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
   </si>
   <si>
     <t xml:space="preserve">No outages (Normal operation).</t>
@@ -2229,79 +2232,79 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2321,7 +2324,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2333,23 +2336,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2357,7 +2360,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2365,15 +2368,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2454,14 +2457,14 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Production"/>
-      <sheetName val="Avg_Pow and Prd Record"/>
+      <sheetName val="Avg_Pow and Prd Chte"/>
+      <sheetName val="Prd_Cht"/>
       <sheetName val="Scrap_CS_MP"/>
-      <sheetName val="Prd_Cht"/>
+      <sheetName val="Dust Handling Cht"/>
+      <sheetName val="DKP_RKF_EFF"/>
       <sheetName val="Feed rate_cht"/>
       <sheetName val="Availability"/>
-      <sheetName val="DKP_RKF_EFF"/>
       <sheetName val=" EFS_EFM"/>
-      <sheetName val="Dust Handling Cht"/>
       <sheetName val="52wks Rolling data"/>
       <sheetName val="Plan vs Actual"/>
       <sheetName val="EF3 Loss"/>
@@ -2494,20 +2497,15 @@
       <sheetName val="EF SHift Data"/>
       <sheetName val="Phys_Availibility"/>
       <sheetName val="Avilability_Data"/>
-      <sheetName val="Data"/>
-      <sheetName val="Avg_Pow_and_Prd_Record"/>
-      <sheetName val="Feed_rate_cht"/>
-      <sheetName val="_EFS_EFM"/>
-      <sheetName val="Dust_Handling_Cht"/>
-      <sheetName val="52wks_Rolling_data"/>
-      <sheetName val="Plan_vs_Actual"/>
-      <sheetName val="EF3_Loss"/>
-      <sheetName val="DKP_SCR_Cht"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="input"/>
       <sheetName val="dBase__3P2"/>
       <sheetName val="_Prod_Cht"/>
       <sheetName val="Power_Utilization"/>
       <sheetName val="Wk_Report_Data"/>
+      <sheetName val="_EFS_EFM"/>
       <sheetName val="EDS_Cht"/>
+      <sheetName val="Dust_Handling_Cht"/>
       <sheetName val="WK_Data_Utilization"/>
       <sheetName val="52_wks_rolling_data"/>
       <sheetName val="2006_Prod_Loss"/>
@@ -2518,6 +2516,12 @@
       <sheetName val="Power_Availability"/>
       <sheetName val="Weekly_Cht_data"/>
       <sheetName val="EF_SHift_Data"/>
+      <sheetName val="Avg_Pow_and_Prd_Chte"/>
+      <sheetName val="Feed_rate_cht"/>
+      <sheetName val="52wks_Rolling_data"/>
+      <sheetName val="Plan_vs_Actual"/>
+      <sheetName val="EF3_Loss"/>
+      <sheetName val="DKP_SCR_Cht"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -2585,375 +2589,13 @@
       <sheetData sheetId="62"/>
       <sheetData sheetId="63"/>
       <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Menu"/>
-      <sheetName val="Page1 of 4"/>
-      <sheetName val="Page2 of 4"/>
-      <sheetName val="Page 3 of 4"/>
-      <sheetName val="Page4 of 4"/>
-      <sheetName val="Data"/>
-      <sheetName val="Module2"/>
-      <sheetName val="Module3"/>
-      <sheetName val="Module1"/>
-      <sheetName val="Table PP"/>
-      <sheetName val="Table Safety"/>
-      <sheetName val="Petea_Q1"/>
-      <sheetName val="Page1_of_4"/>
-      <sheetName val="Page2_of_4"/>
-      <sheetName val="Page_3_of_4"/>
-      <sheetName val="Page4_of_4"/>
-      <sheetName val="Table_PP"/>
-      <sheetName val="Table_Safety"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sulphur Balance"/>
-      <sheetName val="MENU"/>
-      <sheetName val="Data Base PSBU"/>
-      <sheetName val="PRODUCTION"/>
-      <sheetName val="Management Cockpit"/>
-      <sheetName val="2009 OEE"/>
-      <sheetName val="Chart Data1"/>
-      <sheetName val="Prd chart"/>
-      <sheetName val="OPt &amp; PA Cht"/>
-      <sheetName val="Env Chart"/>
-      <sheetName val="%S in Prd "/>
-      <sheetName val="%S in Shipment"/>
-      <sheetName val="%S in Shipment VIJ"/>
-      <sheetName val="Product Off Spec"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="DK EBO"/>
-      <sheetName val="DK WBO"/>
-      <sheetName val="DK TOTAL"/>
-      <sheetName val="Dryer Performance"/>
-      <sheetName val="RKLEDGER"/>
-      <sheetName val="Kiln Performance"/>
-      <sheetName val="EFLEDGER"/>
-      <sheetName val="Fce Performance"/>
-      <sheetName val="CVLEDGER"/>
-      <sheetName val="Inventory"/>
-      <sheetName val="Shortfall Analysis"/>
-      <sheetName val="Recovery New DKp to Prd"/>
-      <sheetName val="Summary of 2006"/>
-      <sheetName val="Recovery New Dusting rate"/>
-      <sheetName val="Recovery EFF to Prd"/>
-      <sheetName val="New Budget 140 Mlbs"/>
-      <sheetName val="Fcast 144 Mlbs"/>
-      <sheetName val="Forecast 150.9 MLbs"/>
-      <sheetName val="Plan vs actual"/>
-      <sheetName val="Act vs F'cast"/>
-      <sheetName val="Forecast 140"/>
-      <sheetName val="2009 Monthly 147 Mlbs"/>
-      <sheetName val="Recovery Analysis"/>
-      <sheetName val="Module1"/>
-      <sheetName val="Forecast 144 MLbs"/>
-      <sheetName val="Forecast"/>
-      <sheetName val="Original Plan_140 MLbs"/>
-      <sheetName val="Recovery"/>
-      <sheetName val="Variance Analysis "/>
-      <sheetName val="New Budget"/>
-      <sheetName val="2009 New Budget"/>
-      <sheetName val="Plan_140 MLbs"/>
-      <sheetName val="Q2 2008 Fcast"/>
-      <sheetName val="Plan_176 MLbs"/>
-      <sheetName val="SPC CHt"/>
-      <sheetName val="Summary Parameter"/>
-      <sheetName val="DK Data"/>
-      <sheetName val="RK Data"/>
-      <sheetName val="EF Data"/>
-      <sheetName val="EF Cht"/>
-      <sheetName val="CV_Data"/>
-      <sheetName val="Chart Data"/>
-      <sheetName val="Env Chat"/>
-      <sheetName val="RK Cht"/>
-      <sheetName val="Bulk Cht"/>
-      <sheetName val="Parameter Cht"/>
-      <sheetName val="Recovery Cht"/>
-      <sheetName val="PARAMETER"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Process Cost Input"/>
-      <sheetName val="Mine Cost Input"/>
-      <sheetName val="Compartment"/>
-      <sheetName val="Blend Grade"/>
-      <sheetName val="Revenue"/>
-      <sheetName val="Ranking"/>
-      <sheetName val="Overall Rank"/>
-      <sheetName val="SS#5 Rank"/>
-      <sheetName val="SS#8 Rank"/>
-      <sheetName val="SS#9 Rank"/>
-      <sheetName val="SS#10 Rank"/>
-      <sheetName val="SS#11 Rank"/>
-      <sheetName val="SS#12 Rank"/>
-      <sheetName val="Feed rate_cht"/>
-      <sheetName val="Availability"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="rev"/>
-      <sheetName val="actual"/>
-      <sheetName val="actual-M"/>
-      <sheetName val="chart"/>
-      <sheetName val="Map"/>
-      <sheetName val="Grade Calculator (2)"/>
-      <sheetName val="CCP2-2Y"/>
-      <sheetName val="historical"/>
-      <sheetName val="Shutdown"/>
-      <sheetName val="Major Shutdown"/>
-      <sheetName val="Reforcast"/>
-      <sheetName val="cpanel"/>
-      <sheetName val="summary"/>
-      <sheetName val="monthly"/>
-      <sheetName val="weekly"/>
-      <sheetName val="bulk-chart"/>
-      <sheetName val="bulk"/>
-      <sheetName val="shipment"/>
-      <sheetName val="oee"/>
-      <sheetName val="2015"/>
-      <sheetName val="2016"/>
-      <sheetName val="Master Schedule"/>
-      <sheetName val="2017"/>
-      <sheetName val="OD OF Historical"/>
-      <sheetName val="EF OF Historical"/>
-      <sheetName val="RK OF Historical"/>
-      <sheetName val="CV OF Historical"/>
-      <sheetName val="Balance"/>
-      <sheetName val="2015Mine"/>
-      <sheetName val="2016Mine"/>
-      <sheetName val="2016Mine-Ori"/>
-      <sheetName val="2017Mine"/>
-      <sheetName val="2017Mine-Ori"/>
-      <sheetName val="Individual"/>
-      <sheetName val="Operating Data"/>
-      <sheetName val="Process Variables"/>
-      <sheetName val="Inv &amp; Comp"/>
-      <sheetName val="Equipment &amp; Dashboard"/>
-      <sheetName val="CCP2-6M"/>
-      <sheetName val="Grade Calculator"/>
-      <sheetName val="check mine"/>
-      <sheetName val="MP_Inv"/>
-      <sheetName val="Scrap_Inv"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Menu"/>
-      <sheetName val="Update_Data"/>
-      <sheetName val="%Op_time"/>
-      <sheetName val="Pow_Set"/>
-      <sheetName val="Avg_Pow"/>
-      <sheetName val="Calcine"/>
-      <sheetName val="EF1_Data"/>
-      <sheetName val="EF2_Data"/>
-      <sheetName val="EF3_Data"/>
-      <sheetName val="EF4_Data"/>
-      <sheetName val="EFT_Data"/>
-      <sheetName val="Plan"/>
-      <sheetName val="2003 MWH_Plan"/>
-      <sheetName val="PRODUCTION"/>
-      <sheetName val="2003_MWH_Plan"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3046,7 +2688,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3075,15 +2717,69 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="PM Schedule Revisi 3"/>
-      <sheetName val="Availability"/>
-      <sheetName val="Compliance"/>
-      <sheetName val="Revision History"/>
-      <sheetName val="lookup"/>
+      <sheetName val="PARAMETER"/>
+      <sheetName val="Summary_Gab"/>
+      <sheetName val="SUMMARY "/>
+      <sheetName val="Plan Monthly"/>
+      <sheetName val="Summary by Hill"/>
+      <sheetName val="West_Yearly"/>
+      <sheetName val="West 1st Half"/>
+      <sheetName val="West 2nd Half"/>
+      <sheetName val="DATA_XXX"/>
+      <sheetName val="Petea_Yearly"/>
+      <sheetName val="Petea_1st Half"/>
+      <sheetName val="Petea_2nd Half"/>
+      <sheetName val="Production Summary"/>
+      <sheetName val="Chart-OB"/>
+      <sheetName val="Chart-ROM"/>
+      <sheetName val="Chart-SSP"/>
+      <sheetName val="Chart-OB(W) Distribution"/>
+      <sheetName val="Chart-OB(E) Distribution"/>
+      <sheetName val="Chart-ROM (W) Distribution"/>
+      <sheetName val="Chart-ROM (E) Distribution"/>
+      <sheetName val="Monthly_Ni"/>
+      <sheetName val="Monthly_Fe"/>
+      <sheetName val="Monthly_SM"/>
+      <sheetName val="Monthly_Co"/>
+      <sheetName val="Monthly_SR"/>
+      <sheetName val="Monthly_Civil"/>
+      <sheetName val="Monthly_DKP Prod"/>
+      <sheetName val="Monthly_WOS Stat"/>
+      <sheetName val="Monthly_LBS Ni"/>
+      <sheetName val="OB_Distance"/>
+      <sheetName val="ROM_Distance"/>
+      <sheetName val="SSP_Distance"/>
+      <sheetName val="Quarry_Distance"/>
+      <sheetName val="SS#5_Prod"/>
+      <sheetName val="SS#8_Prod"/>
+      <sheetName val="SS#9_Prod"/>
+      <sheetName val="SS#11_Prod"/>
+      <sheetName val="SS#10_Pet"/>
+      <sheetName val="SS#All"/>
+      <sheetName val="Ni_Grade"/>
+      <sheetName val="Fe_Grade"/>
+      <sheetName val="SM_Ratio"/>
+      <sheetName val="Chart-OB by Hill"/>
+      <sheetName val="Chart-ROM by Hill"/>
+      <sheetName val="Chart-Civil by Hill"/>
+      <sheetName val="Chart-SSP by Hill"/>
+      <sheetName val="Chart-OREX by Hill"/>
+      <sheetName val="Chart-DKP by Hill"/>
+      <sheetName val="Chart-lbs by hill"/>
+      <sheetName val="Update_Data"/>
+      <sheetName val="%Op_time"/>
+      <sheetName val="EF1_Data"/>
+      <sheetName val="Pow_Set"/>
+      <sheetName val="EF2_Data"/>
+      <sheetName val="Avg_Pow"/>
+      <sheetName val="EF3_Data"/>
+      <sheetName val="Calcine"/>
+      <sheetName val="EF4_Data"/>
+      <sheetName val="EFT_Data"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -3091,12 +2787,66 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3421,328 +3171,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="P Plant"/>
-      <sheetName val="SUMMARY "/>
-      <sheetName val="petea_(2007)"/>
-      <sheetName val="west_(2007)"/>
-      <sheetName val="west_Q1"/>
-      <sheetName val="west_Q2"/>
-      <sheetName val="west_Q3"/>
-      <sheetName val="west_Q4"/>
-      <sheetName val="Petea_Q1"/>
-      <sheetName val="Petea_Q2"/>
-      <sheetName val="Petea_Q3"/>
-      <sheetName val="Petea_Q4"/>
-      <sheetName val="strategy"/>
-      <sheetName val="Wk_Press data"/>
-      <sheetName val="Detailed Data Capture"/>
-      <sheetName val="P_Plant"/>
-      <sheetName val="SUMMARY_"/>
-      <sheetName val="Wk_Press_data"/>
-      <sheetName val="Detailed_Data_Capture"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PARAMETER"/>
-      <sheetName val="Summary_Gab"/>
-      <sheetName val="SUMMARY "/>
-      <sheetName val="Plan Monthly"/>
-      <sheetName val="Summary by Hill"/>
-      <sheetName val="West_Yearly"/>
-      <sheetName val="West 1st Half"/>
-      <sheetName val="West 2nd Half"/>
-      <sheetName val="DATA_XXX"/>
-      <sheetName val="Petea_Yearly"/>
-      <sheetName val="Petea_1st Half"/>
-      <sheetName val="Petea_2nd Half"/>
-      <sheetName val="Production Summary"/>
-      <sheetName val="Chart-OB"/>
-      <sheetName val="Chart-ROM"/>
-      <sheetName val="Chart-SSP"/>
-      <sheetName val="Chart-OB(W) Distribution"/>
-      <sheetName val="Chart-OB(E) Distribution"/>
-      <sheetName val="Chart-ROM (W) Distribution"/>
-      <sheetName val="Chart-ROM (E) Distribution"/>
-      <sheetName val="Monthly_Ni"/>
-      <sheetName val="Monthly_Fe"/>
-      <sheetName val="Monthly_SM"/>
-      <sheetName val="Monthly_Co"/>
-      <sheetName val="Monthly_SR"/>
-      <sheetName val="Monthly_Civil"/>
-      <sheetName val="Monthly_DKP Prod"/>
-      <sheetName val="Monthly_WOS Stat"/>
-      <sheetName val="Monthly_LBS Ni"/>
-      <sheetName val="OB_Distance"/>
-      <sheetName val="ROM_Distance"/>
-      <sheetName val="SSP_Distance"/>
-      <sheetName val="Quarry_Distance"/>
-      <sheetName val="SS#5_Prod"/>
-      <sheetName val="SS#8_Prod"/>
-      <sheetName val="SS#9_Prod"/>
-      <sheetName val="SS#11_Prod"/>
-      <sheetName val="SS#10_Pet"/>
-      <sheetName val="SS#All"/>
-      <sheetName val="Ni_Grade"/>
-      <sheetName val="Fe_Grade"/>
-      <sheetName val="SM_Ratio"/>
-      <sheetName val="Chart-OB by Hill"/>
-      <sheetName val="Chart-ROM by Hill"/>
-      <sheetName val="Chart-Civil by Hill"/>
-      <sheetName val="Chart-SSP by Hill"/>
-      <sheetName val="Chart-OREX by Hill"/>
-      <sheetName val="Chart-DKP by Hill"/>
-      <sheetName val="Chart-lbs by hill"/>
-      <sheetName val="Update_Data"/>
-      <sheetName val="%Op_time"/>
-      <sheetName val="EF1_Data"/>
-      <sheetName val="Pow_Set"/>
-      <sheetName val="EF2_Data"/>
-      <sheetName val="Avg_Pow"/>
-      <sheetName val="EF3_Data"/>
-      <sheetName val="Calcine"/>
-      <sheetName val="EF4_Data"/>
-      <sheetName val="EFT_Data"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Production"/>
-      <sheetName val="Avg_Pow and Prd Chte"/>
-      <sheetName val="Prd_Cht"/>
-      <sheetName val="Scrap_CS_MP"/>
-      <sheetName val="Dust Handling Cht"/>
-      <sheetName val="DKP_RKF_EFF"/>
-      <sheetName val="Feed rate_cht"/>
-      <sheetName val="Availability"/>
-      <sheetName val=" EFS_EFM"/>
-      <sheetName val="52wks Rolling data"/>
-      <sheetName val="Plan vs Actual"/>
-      <sheetName val="EF3 Loss"/>
-      <sheetName val="DK_Delay"/>
-      <sheetName val="RK_Delay"/>
-      <sheetName val="CT_Delay"/>
-      <sheetName val="EF_Delay"/>
-      <sheetName val="Power&gt;80%"/>
-      <sheetName val="DKP SCR_Cht"/>
-      <sheetName val="WP_Menu"/>
-      <sheetName val="WK_Balance"/>
-      <sheetName val="dBase _3P2"/>
-      <sheetName val="Index_Data"/>
-      <sheetName val=" Prod Cht"/>
-      <sheetName val="Recovery"/>
-      <sheetName val="Power Utilization"/>
-      <sheetName val="Wk_Report Data"/>
-      <sheetName val="EDS Cht"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="WK Data Utilization"/>
-      <sheetName val="52 wks rolling data"/>
-      <sheetName val="2006 Prod Loss"/>
-      <sheetName val="DK EDS"/>
-      <sheetName val="RK EDS"/>
-      <sheetName val="CT_EDS"/>
-      <sheetName val="EF EDS"/>
-      <sheetName val="2004 Prd Loss"/>
-      <sheetName val="Power Availability"/>
-      <sheetName val="Weekly Cht_data"/>
-      <sheetName val="EF SHift Data"/>
-      <sheetName val="Phys_Availibility"/>
-      <sheetName val="Avilability_Data"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="input"/>
-      <sheetName val="dBase__3P2"/>
-      <sheetName val="_Prod_Cht"/>
-      <sheetName val="Power_Utilization"/>
-      <sheetName val="Wk_Report_Data"/>
-      <sheetName val="_EFS_EFM"/>
-      <sheetName val="EDS_Cht"/>
-      <sheetName val="Dust_Handling_Cht"/>
-      <sheetName val="WK_Data_Utilization"/>
-      <sheetName val="52_wks_rolling_data"/>
-      <sheetName val="2006_Prod_Loss"/>
-      <sheetName val="DK_EDS"/>
-      <sheetName val="RK_EDS"/>
-      <sheetName val="EF_EDS"/>
-      <sheetName val="2004_Prd_Loss"/>
-      <sheetName val="Power_Availability"/>
-      <sheetName val="Weekly_Cht_data"/>
-      <sheetName val="EF_SHift_Data"/>
-      <sheetName val="Avg_Pow_and_Prd_Chte"/>
-      <sheetName val="Feed_rate_cht"/>
-      <sheetName val="52wks_Rolling_data"/>
-      <sheetName val="Plan_vs_Actual"/>
-      <sheetName val="EF3_Loss"/>
-      <sheetName val="DKP_SCR_Cht"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3779,7 +3208,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3908,19 +3337,28 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Menu"/>
+      <sheetName val="Page1 of 4"/>
+      <sheetName val="Page2 of 4"/>
+      <sheetName val="Page 3 of 4"/>
+      <sheetName val="Page4 of 4"/>
       <sheetName val="Data"/>
-      <sheetName val="CS Asay_Cht"/>
-      <sheetName val="CS_Inv_cht"/>
-      <sheetName val="Scrap_Inv"/>
-      <sheetName val="MP_Inv"/>
-      <sheetName val="CHT_Data"/>
-      <sheetName val="EBO"/>
-      <sheetName val="CS_Asay_Cht"/>
+      <sheetName val="Module2"/>
+      <sheetName val="Module3"/>
+      <sheetName val="Module1"/>
+      <sheetName val="Table PP"/>
+      <sheetName val="Table Safety"/>
+      <sheetName val="Petea_Q1"/>
+      <sheetName val="Page1_of_4"/>
+      <sheetName val="Page2_of_4"/>
+      <sheetName val="Page_3_of_4"/>
+      <sheetName val="Page4_of_4"/>
+      <sheetName val="Table_PP"/>
+      <sheetName val="Table_Safety"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -3932,6 +3370,352 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sulphur Balance"/>
+      <sheetName val="MENU"/>
+      <sheetName val="Data Base PSBU"/>
+      <sheetName val="PRODUCTION"/>
+      <sheetName val="Management Cockpit"/>
+      <sheetName val="2009 OEE"/>
+      <sheetName val="Chart Data1"/>
+      <sheetName val="Prd chart"/>
+      <sheetName val="OPt &amp; PA Cht"/>
+      <sheetName val="Env Chart"/>
+      <sheetName val="%S in Prd "/>
+      <sheetName val="%S in Shipment"/>
+      <sheetName val="%S in Shipment VIJ"/>
+      <sheetName val="Product Off Spec"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="DK EBO"/>
+      <sheetName val="DK WBO"/>
+      <sheetName val="DK TOTAL"/>
+      <sheetName val="Dryer Performance"/>
+      <sheetName val="RKLEDGER"/>
+      <sheetName val="Kiln Performance"/>
+      <sheetName val="EFLEDGER"/>
+      <sheetName val="Fce Performance"/>
+      <sheetName val="CVLEDGER"/>
+      <sheetName val="Inventory"/>
+      <sheetName val="Shortfall Analysis"/>
+      <sheetName val="Recovery New DKp to Prd"/>
+      <sheetName val="Summary of 2006"/>
+      <sheetName val="Recovery New Dusting rate"/>
+      <sheetName val="Recovery EFF to Prd"/>
+      <sheetName val="New Budget 140 Mlbs"/>
+      <sheetName val="Fcast 144 Mlbs"/>
+      <sheetName val="Forecast 150.9 MLbs"/>
+      <sheetName val="Plan vs actual"/>
+      <sheetName val="Act vs F'cast"/>
+      <sheetName val="Forecast 140"/>
+      <sheetName val="2009 Monthly 147 Mlbs"/>
+      <sheetName val="Recovery Analysis"/>
+      <sheetName val="Module1"/>
+      <sheetName val="Forecast 144 MLbs"/>
+      <sheetName val="Forecast"/>
+      <sheetName val="Original Plan_140 MLbs"/>
+      <sheetName val="Recovery"/>
+      <sheetName val="Variance Analysis "/>
+      <sheetName val="New Budget"/>
+      <sheetName val="2009 New Budget"/>
+      <sheetName val="Plan_140 MLbs"/>
+      <sheetName val="Q2 2008 Fcast"/>
+      <sheetName val="Plan_176 MLbs"/>
+      <sheetName val="SPC CHt"/>
+      <sheetName val="Summary Parameter"/>
+      <sheetName val="DK Data"/>
+      <sheetName val="RK Data"/>
+      <sheetName val="EF Data"/>
+      <sheetName val="EF Cht"/>
+      <sheetName val="CV_Data"/>
+      <sheetName val="Chart Data"/>
+      <sheetName val="Env Chat"/>
+      <sheetName val="RK Cht"/>
+      <sheetName val="Bulk Cht"/>
+      <sheetName val="Parameter Cht"/>
+      <sheetName val="Recovery Cht"/>
+      <sheetName val="PARAMETER"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Process Cost Input"/>
+      <sheetName val="Mine Cost Input"/>
+      <sheetName val="Compartment"/>
+      <sheetName val="Blend Grade"/>
+      <sheetName val="Revenue"/>
+      <sheetName val="Ranking"/>
+      <sheetName val="Overall Rank"/>
+      <sheetName val="SS#5 Rank"/>
+      <sheetName val="SS#8 Rank"/>
+      <sheetName val="SS#9 Rank"/>
+      <sheetName val="SS#10 Rank"/>
+      <sheetName val="SS#11 Rank"/>
+      <sheetName val="SS#12 Rank"/>
+      <sheetName val="Feed rate_cht"/>
+      <sheetName val="Availability"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="PM Schedule Revisi 3"/>
+      <sheetName val="Availability"/>
+      <sheetName val="Compliance"/>
+      <sheetName val="Revision History"/>
+      <sheetName val="lookup"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="rev"/>
+      <sheetName val="actual"/>
+      <sheetName val="actual-M"/>
+      <sheetName val="chart"/>
+      <sheetName val="Map"/>
+      <sheetName val="Grade Calculator (2)"/>
+      <sheetName val="CCP2-2Y"/>
+      <sheetName val="historical"/>
+      <sheetName val="Shutdown"/>
+      <sheetName val="Major Shutdown"/>
+      <sheetName val="Reforcast"/>
+      <sheetName val="cpanel"/>
+      <sheetName val="summary"/>
+      <sheetName val="monthly"/>
+      <sheetName val="weekly"/>
+      <sheetName val="bulk-chart"/>
+      <sheetName val="bulk"/>
+      <sheetName val="shipment"/>
+      <sheetName val="oee"/>
+      <sheetName val="2015"/>
+      <sheetName val="2016"/>
+      <sheetName val="Master Schedule"/>
+      <sheetName val="2017"/>
+      <sheetName val="OD OF Historical"/>
+      <sheetName val="EF OF Historical"/>
+      <sheetName val="RK OF Historical"/>
+      <sheetName val="CV OF Historical"/>
+      <sheetName val="Balance"/>
+      <sheetName val="2015Mine"/>
+      <sheetName val="2016Mine"/>
+      <sheetName val="2016Mine-Ori"/>
+      <sheetName val="2017Mine"/>
+      <sheetName val="2017Mine-Ori"/>
+      <sheetName val="Individual"/>
+      <sheetName val="Operating Data"/>
+      <sheetName val="Process Variables"/>
+      <sheetName val="Inv &amp; Comp"/>
+      <sheetName val="Equipment &amp; Dashboard"/>
+      <sheetName val="CCP2-6M"/>
+      <sheetName val="Grade Calculator"/>
+      <sheetName val="check mine"/>
+      <sheetName val="MP_Inv"/>
+      <sheetName val="Scrap_Inv"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Menu"/>
+      <sheetName val="Update_Data"/>
+      <sheetName val="%Op_time"/>
+      <sheetName val="Pow_Set"/>
+      <sheetName val="Avg_Pow"/>
+      <sheetName val="Calcine"/>
+      <sheetName val="EF1_Data"/>
+      <sheetName val="EF2_Data"/>
+      <sheetName val="EF3_Data"/>
+      <sheetName val="EF4_Data"/>
+      <sheetName val="EFT_Data"/>
+      <sheetName val="Plan"/>
+      <sheetName val="2003 MWH_Plan"/>
+      <sheetName val="PRODUCTION"/>
+      <sheetName val="2003_MWH_Plan"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -26444,10 +26228,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1048576"/>
+  <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A328" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E377" activeCellId="0" sqref="E377"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26460,7 +26244,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="19" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -26514,6 +26298,18 @@
       </c>
       <c r="R1" s="36" t="s">
         <v>89</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26566,7 +26362,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26619,7 +26415,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26672,7 +26468,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26725,7 +26521,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26778,7 +26574,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26831,7 +26627,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26884,7 +26680,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26937,7 +26733,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26990,7 +26786,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27043,7 +26839,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="33" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27096,7 +26892,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27149,7 +26945,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27202,7 +26998,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27255,7 +27051,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27308,7 +27104,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27361,7 +27157,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27414,7 +27210,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="33" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27467,7 +27263,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="33" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27520,7 +27316,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27573,7 +27369,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27626,7 +27422,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="33" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27679,7 +27475,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27732,7 +27528,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27785,7 +27581,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27838,7 +27634,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="33" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27891,7 +27687,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27944,7 +27740,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27997,7 +27793,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="33" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28050,7 +27846,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="33" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28103,7 +27899,7 @@
         <v>0</v>
       </c>
       <c r="Q31" s="33" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28156,7 +27952,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28209,7 +28005,7 @@
         <v>0</v>
       </c>
       <c r="Q33" s="33" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28262,7 +28058,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="33" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28315,7 +28111,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28368,7 +28164,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28421,7 +28217,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28474,7 +28270,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28527,7 +28323,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="33" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28580,7 +28376,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="33" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28633,7 +28429,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="33" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28686,7 +28482,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28739,7 +28535,7 @@
         <v>0</v>
       </c>
       <c r="Q43" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28792,7 +28588,7 @@
         <v>0</v>
       </c>
       <c r="Q44" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28845,7 +28641,7 @@
         <v>0</v>
       </c>
       <c r="Q45" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28898,7 +28694,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28951,7 +28747,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29004,7 +28800,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29057,7 +28853,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29110,7 +28906,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29163,7 +28959,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="157.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29216,7 +29012,7 @@
         <v>0</v>
       </c>
       <c r="Q52" s="33" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29269,7 +29065,7 @@
         <v>0</v>
       </c>
       <c r="Q53" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29322,7 +29118,7 @@
         <v>0</v>
       </c>
       <c r="Q54" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29375,7 +29171,7 @@
         <v>0</v>
       </c>
       <c r="Q55" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29428,7 +29224,7 @@
         <v>0</v>
       </c>
       <c r="Q56" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29481,7 +29277,7 @@
         <v>0</v>
       </c>
       <c r="Q57" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29534,7 +29330,7 @@
         <v>0</v>
       </c>
       <c r="Q58" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29587,7 +29383,7 @@
         <v>0</v>
       </c>
       <c r="Q59" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29640,7 +29436,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="33" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29693,7 +29489,7 @@
         <v>0</v>
       </c>
       <c r="Q61" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29746,7 +29542,7 @@
         <v>0</v>
       </c>
       <c r="Q62" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29799,7 +29595,7 @@
         <v>0</v>
       </c>
       <c r="Q63" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29852,7 +29648,7 @@
         <v>0</v>
       </c>
       <c r="Q64" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29905,7 +29701,7 @@
         <v>0</v>
       </c>
       <c r="Q65" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29958,7 +29754,7 @@
         <v>0</v>
       </c>
       <c r="Q66" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30011,7 +29807,7 @@
         <v>0</v>
       </c>
       <c r="Q67" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30064,7 +29860,7 @@
         <v>0</v>
       </c>
       <c r="Q68" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30117,7 +29913,7 @@
         <v>0</v>
       </c>
       <c r="Q69" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30170,7 +29966,7 @@
         <v>0</v>
       </c>
       <c r="Q70" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30223,7 +30019,7 @@
         <v>0</v>
       </c>
       <c r="Q71" s="33" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30276,7 +30072,7 @@
         <v>0</v>
       </c>
       <c r="Q72" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30329,7 +30125,7 @@
         <v>0</v>
       </c>
       <c r="Q73" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30382,7 +30178,7 @@
         <v>0</v>
       </c>
       <c r="Q74" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30435,7 +30231,7 @@
         <v>0</v>
       </c>
       <c r="Q75" s="33" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30488,7 +30284,7 @@
         <v>0</v>
       </c>
       <c r="Q76" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30541,7 +30337,7 @@
         <v>0</v>
       </c>
       <c r="Q77" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30594,7 +30390,7 @@
         <v>0</v>
       </c>
       <c r="Q78" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30647,7 +30443,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30700,7 +30496,7 @@
         <v>0</v>
       </c>
       <c r="Q80" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30753,7 +30549,7 @@
         <v>0</v>
       </c>
       <c r="Q81" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30806,7 +30602,7 @@
         <v>0</v>
       </c>
       <c r="Q82" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30859,7 +30655,7 @@
         <v>0</v>
       </c>
       <c r="Q83" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30912,7 +30708,7 @@
         <v>0</v>
       </c>
       <c r="Q84" s="33" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30965,7 +30761,7 @@
         <v>0</v>
       </c>
       <c r="Q85" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31018,7 +30814,7 @@
         <v>0</v>
       </c>
       <c r="Q86" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31071,7 +30867,7 @@
         <v>0</v>
       </c>
       <c r="Q87" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31124,7 +30920,7 @@
         <v>0</v>
       </c>
       <c r="Q88" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31177,7 +30973,7 @@
         <v>0</v>
       </c>
       <c r="Q89" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31230,7 +31026,7 @@
         <v>0</v>
       </c>
       <c r="Q90" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31283,7 +31079,7 @@
         <v>0</v>
       </c>
       <c r="Q91" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31336,7 +31132,7 @@
         <v>0</v>
       </c>
       <c r="Q92" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31389,7 +31185,7 @@
         <v>0</v>
       </c>
       <c r="Q93" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31442,7 +31238,7 @@
         <v>0</v>
       </c>
       <c r="Q94" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31495,7 +31291,7 @@
         <v>0</v>
       </c>
       <c r="Q95" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31548,7 +31344,7 @@
         <v>0</v>
       </c>
       <c r="Q96" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31601,7 +31397,7 @@
         <v>0</v>
       </c>
       <c r="Q97" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31654,7 +31450,7 @@
         <v>0</v>
       </c>
       <c r="Q98" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31707,7 +31503,7 @@
         <v>0</v>
       </c>
       <c r="Q99" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31760,7 +31556,7 @@
         <v>0</v>
       </c>
       <c r="Q100" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31813,7 +31609,7 @@
         <v>0</v>
       </c>
       <c r="Q101" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31866,7 +31662,7 @@
         <v>0</v>
       </c>
       <c r="Q102" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31919,7 +31715,7 @@
         <v>0</v>
       </c>
       <c r="Q103" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31972,7 +31768,7 @@
         <v>0</v>
       </c>
       <c r="Q104" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32025,7 +31821,7 @@
         <v>0</v>
       </c>
       <c r="Q105" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32078,7 +31874,7 @@
         <v>0</v>
       </c>
       <c r="Q106" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32131,7 +31927,7 @@
         <v>0</v>
       </c>
       <c r="Q107" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32184,7 +31980,7 @@
         <v>0</v>
       </c>
       <c r="Q108" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32237,7 +32033,7 @@
         <v>0</v>
       </c>
       <c r="Q109" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32290,7 +32086,7 @@
         <v>0</v>
       </c>
       <c r="Q110" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32343,7 +32139,7 @@
         <v>0</v>
       </c>
       <c r="Q111" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32396,7 +32192,7 @@
         <v>0</v>
       </c>
       <c r="Q112" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32449,7 +32245,7 @@
         <v>0</v>
       </c>
       <c r="Q113" s="33" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32502,7 +32298,7 @@
         <v>0</v>
       </c>
       <c r="Q114" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32555,7 +32351,7 @@
         <v>0</v>
       </c>
       <c r="Q115" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32608,7 +32404,7 @@
         <v>0</v>
       </c>
       <c r="Q116" s="33" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32661,7 +32457,7 @@
         <v>0</v>
       </c>
       <c r="Q117" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32714,7 +32510,7 @@
         <v>0</v>
       </c>
       <c r="Q118" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32767,7 +32563,7 @@
         <v>0</v>
       </c>
       <c r="Q119" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32820,7 +32616,7 @@
         <v>0</v>
       </c>
       <c r="Q120" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32873,7 +32669,7 @@
         <v>0</v>
       </c>
       <c r="Q121" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32926,7 +32722,7 @@
         <v>0</v>
       </c>
       <c r="Q122" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32979,7 +32775,7 @@
         <v>0</v>
       </c>
       <c r="Q123" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33032,7 +32828,7 @@
         <v>0</v>
       </c>
       <c r="Q124" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33085,7 +32881,7 @@
         <v>0</v>
       </c>
       <c r="Q125" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33138,7 +32934,7 @@
         <v>0</v>
       </c>
       <c r="Q126" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33191,7 +32987,7 @@
         <v>0</v>
       </c>
       <c r="Q127" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33244,7 +33040,7 @@
         <v>0</v>
       </c>
       <c r="Q128" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33297,7 +33093,7 @@
         <v>0</v>
       </c>
       <c r="Q129" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33350,7 +33146,7 @@
         <v>0</v>
       </c>
       <c r="Q130" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33403,7 +33199,7 @@
         <v>0</v>
       </c>
       <c r="Q131" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33456,7 +33252,7 @@
         <v>0</v>
       </c>
       <c r="Q132" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33509,7 +33305,7 @@
         <v>0</v>
       </c>
       <c r="Q133" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33562,7 +33358,7 @@
         <v>0</v>
       </c>
       <c r="Q134" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33615,7 +33411,7 @@
         <v>0</v>
       </c>
       <c r="Q135" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33668,7 +33464,7 @@
         <v>0</v>
       </c>
       <c r="Q136" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33721,7 +33517,7 @@
         <v>0</v>
       </c>
       <c r="Q137" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33774,7 +33570,7 @@
         <v>0</v>
       </c>
       <c r="Q138" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33827,7 +33623,7 @@
         <v>0</v>
       </c>
       <c r="Q139" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33880,7 +33676,7 @@
         <v>0</v>
       </c>
       <c r="Q140" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33933,7 +33729,7 @@
         <v>0</v>
       </c>
       <c r="Q141" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33986,7 +33782,7 @@
         <v>0</v>
       </c>
       <c r="Q142" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34039,7 +33835,7 @@
         <v>0</v>
       </c>
       <c r="Q143" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34092,7 +33888,7 @@
         <v>0</v>
       </c>
       <c r="Q144" s="33" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34145,7 +33941,7 @@
         <v>0</v>
       </c>
       <c r="Q145" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34198,7 +33994,7 @@
         <v>0</v>
       </c>
       <c r="Q146" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34251,7 +34047,7 @@
         <v>0</v>
       </c>
       <c r="Q147" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34304,7 +34100,7 @@
         <v>0</v>
       </c>
       <c r="Q148" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34357,7 +34153,7 @@
         <v>0</v>
       </c>
       <c r="Q149" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34410,7 +34206,7 @@
         <v>0</v>
       </c>
       <c r="Q150" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34463,7 +34259,7 @@
         <v>0</v>
       </c>
       <c r="Q151" s="33" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34516,7 +34312,7 @@
         <v>0</v>
       </c>
       <c r="Q152" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34569,7 +34365,7 @@
         <v>0</v>
       </c>
       <c r="Q153" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34622,7 +34418,7 @@
         <v>0</v>
       </c>
       <c r="Q154" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34675,7 +34471,7 @@
         <v>0</v>
       </c>
       <c r="Q155" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34728,7 +34524,7 @@
         <v>0</v>
       </c>
       <c r="Q156" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34781,7 +34577,7 @@
         <v>0</v>
       </c>
       <c r="Q157" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34834,7 +34630,7 @@
         <v>0</v>
       </c>
       <c r="Q158" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34887,7 +34683,7 @@
         <v>0</v>
       </c>
       <c r="Q159" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34940,7 +34736,7 @@
         <v>0</v>
       </c>
       <c r="Q160" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34993,7 +34789,7 @@
         <v>0</v>
       </c>
       <c r="Q161" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35046,7 +34842,7 @@
         <v>0</v>
       </c>
       <c r="Q162" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35099,7 +34895,7 @@
         <v>0</v>
       </c>
       <c r="Q163" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35152,7 +34948,7 @@
         <v>0</v>
       </c>
       <c r="Q164" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35205,7 +35001,7 @@
         <v>0</v>
       </c>
       <c r="Q165" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35258,7 +35054,7 @@
         <v>0</v>
       </c>
       <c r="Q166" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35311,7 +35107,7 @@
         <v>0</v>
       </c>
       <c r="Q167" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35364,7 +35160,7 @@
         <v>0</v>
       </c>
       <c r="Q168" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35417,7 +35213,7 @@
         <v>0</v>
       </c>
       <c r="Q169" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35470,7 +35266,7 @@
         <v>0</v>
       </c>
       <c r="Q170" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35523,7 +35319,7 @@
         <v>0</v>
       </c>
       <c r="Q171" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35576,7 +35372,7 @@
         <v>0</v>
       </c>
       <c r="Q172" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35629,7 +35425,7 @@
         <v>0</v>
       </c>
       <c r="Q173" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35682,7 +35478,7 @@
         <v>0</v>
       </c>
       <c r="Q174" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35735,7 +35531,7 @@
         <v>0</v>
       </c>
       <c r="Q175" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35788,7 +35584,7 @@
         <v>0</v>
       </c>
       <c r="Q176" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35841,7 +35637,7 @@
         <v>0</v>
       </c>
       <c r="Q177" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35894,7 +35690,7 @@
         <v>0</v>
       </c>
       <c r="Q178" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35947,7 +35743,7 @@
         <v>0</v>
       </c>
       <c r="Q179" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36000,7 +35796,7 @@
         <v>0</v>
       </c>
       <c r="Q180" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36053,7 +35849,7 @@
         <v>0</v>
       </c>
       <c r="Q181" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36106,7 +35902,7 @@
         <v>0</v>
       </c>
       <c r="Q182" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36159,7 +35955,7 @@
         <v>0</v>
       </c>
       <c r="Q183" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36212,7 +36008,7 @@
         <v>0</v>
       </c>
       <c r="Q184" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36265,7 +36061,7 @@
         <v>0</v>
       </c>
       <c r="Q185" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36318,7 +36114,7 @@
         <v>0</v>
       </c>
       <c r="Q186" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36371,7 +36167,7 @@
         <v>0</v>
       </c>
       <c r="Q187" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36424,7 +36220,7 @@
         <v>0</v>
       </c>
       <c r="Q188" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36477,7 +36273,7 @@
         <v>0</v>
       </c>
       <c r="Q189" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36530,7 +36326,7 @@
         <v>0</v>
       </c>
       <c r="Q190" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36583,7 +36379,7 @@
         <v>0</v>
       </c>
       <c r="Q191" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36636,7 +36432,7 @@
         <v>0</v>
       </c>
       <c r="Q192" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36689,7 +36485,7 @@
         <v>0</v>
       </c>
       <c r="Q193" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36742,7 +36538,7 @@
         <v>0</v>
       </c>
       <c r="Q194" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36795,7 +36591,7 @@
         <v>0</v>
       </c>
       <c r="Q195" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36848,7 +36644,7 @@
         <v>0</v>
       </c>
       <c r="Q196" s="33" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36901,7 +36697,7 @@
         <v>0</v>
       </c>
       <c r="Q197" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36954,7 +36750,7 @@
         <v>0</v>
       </c>
       <c r="Q198" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37007,7 +36803,7 @@
         <v>0</v>
       </c>
       <c r="Q199" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37060,7 +36856,7 @@
         <v>0</v>
       </c>
       <c r="Q200" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37113,7 +36909,7 @@
         <v>0</v>
       </c>
       <c r="Q201" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37166,7 +36962,7 @@
         <v>0</v>
       </c>
       <c r="Q202" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="56.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37219,7 +37015,7 @@
         <v>0</v>
       </c>
       <c r="Q203" s="33" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37272,7 +37068,7 @@
         <v>0</v>
       </c>
       <c r="Q204" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37325,7 +37121,7 @@
         <v>0</v>
       </c>
       <c r="Q205" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37378,7 +37174,7 @@
         <v>0</v>
       </c>
       <c r="Q206" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37431,7 +37227,7 @@
         <v>0</v>
       </c>
       <c r="Q207" s="33" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37484,7 +37280,7 @@
         <v>0</v>
       </c>
       <c r="Q208" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37537,7 +37333,7 @@
         <v>0</v>
       </c>
       <c r="Q209" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37590,7 +37386,7 @@
         <v>0</v>
       </c>
       <c r="Q210" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37643,7 +37439,7 @@
         <v>0</v>
       </c>
       <c r="Q211" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37696,7 +37492,7 @@
         <v>0</v>
       </c>
       <c r="Q212" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37749,7 +37545,7 @@
         <v>0</v>
       </c>
       <c r="Q213" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37802,7 +37598,7 @@
         <v>0</v>
       </c>
       <c r="Q214" s="33" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37855,7 +37651,7 @@
         <v>0</v>
       </c>
       <c r="Q215" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37908,7 +37704,7 @@
         <v>0</v>
       </c>
       <c r="Q216" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37961,7 +37757,7 @@
         <v>0</v>
       </c>
       <c r="Q217" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38014,7 +37810,7 @@
         <v>0</v>
       </c>
       <c r="Q218" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38067,7 +37863,7 @@
         <v>0</v>
       </c>
       <c r="Q219" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38120,7 +37916,7 @@
         <v>0</v>
       </c>
       <c r="Q220" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38173,7 +37969,7 @@
         <v>0</v>
       </c>
       <c r="Q221" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38226,7 +38022,7 @@
         <v>0</v>
       </c>
       <c r="Q222" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38279,7 +38075,7 @@
         <v>0</v>
       </c>
       <c r="Q223" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38332,7 +38128,7 @@
         <v>0</v>
       </c>
       <c r="Q224" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38385,7 +38181,7 @@
         <v>0</v>
       </c>
       <c r="Q225" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38438,7 +38234,7 @@
         <v>0</v>
       </c>
       <c r="Q226" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38491,7 +38287,7 @@
         <v>0</v>
       </c>
       <c r="Q227" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38544,7 +38340,7 @@
         <v>0</v>
       </c>
       <c r="Q228" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38597,7 +38393,7 @@
         <v>0</v>
       </c>
       <c r="Q229" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38650,7 +38446,7 @@
         <v>0</v>
       </c>
       <c r="Q230" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38703,7 +38499,7 @@
         <v>0</v>
       </c>
       <c r="Q231" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38756,7 +38552,7 @@
         <v>0</v>
       </c>
       <c r="Q232" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38809,7 +38605,7 @@
         <v>0</v>
       </c>
       <c r="Q233" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38862,7 +38658,7 @@
         <v>0</v>
       </c>
       <c r="Q234" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38915,7 +38711,7 @@
         <v>0</v>
       </c>
       <c r="Q235" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38968,7 +38764,7 @@
         <v>0</v>
       </c>
       <c r="Q236" s="33" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39021,7 +38817,7 @@
         <v>0</v>
       </c>
       <c r="Q237" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39074,7 +38870,7 @@
         <v>0</v>
       </c>
       <c r="Q238" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39127,7 +38923,7 @@
         <v>0</v>
       </c>
       <c r="Q239" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39180,7 +38976,7 @@
         <v>0</v>
       </c>
       <c r="Q240" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39233,7 +39029,7 @@
         <v>0</v>
       </c>
       <c r="Q241" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39286,7 +39082,7 @@
         <v>0</v>
       </c>
       <c r="Q242" s="33" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39339,7 +39135,7 @@
         <v>0</v>
       </c>
       <c r="Q243" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39392,7 +39188,7 @@
         <v>0</v>
       </c>
       <c r="Q244" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39445,7 +39241,7 @@
         <v>0</v>
       </c>
       <c r="Q245" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39498,7 +39294,7 @@
         <v>0</v>
       </c>
       <c r="Q246" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39551,7 +39347,7 @@
         <v>0</v>
       </c>
       <c r="Q247" s="33" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39604,7 +39400,7 @@
         <v>0</v>
       </c>
       <c r="Q248" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39657,7 +39453,7 @@
         <v>0</v>
       </c>
       <c r="Q249" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39710,7 +39506,7 @@
         <v>0</v>
       </c>
       <c r="Q250" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39763,7 +39559,7 @@
         <v>0</v>
       </c>
       <c r="Q251" s="33" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39816,7 +39612,7 @@
         <v>0</v>
       </c>
       <c r="Q252" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39869,7 +39665,7 @@
         <v>0</v>
       </c>
       <c r="Q253" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39922,7 +39718,7 @@
         <v>0</v>
       </c>
       <c r="Q254" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39975,7 +39771,7 @@
         <v>0</v>
       </c>
       <c r="Q255" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40028,7 +39824,7 @@
         <v>0</v>
       </c>
       <c r="Q256" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40081,7 +39877,7 @@
         <v>0</v>
       </c>
       <c r="Q257" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40134,7 +39930,7 @@
         <v>0</v>
       </c>
       <c r="Q258" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40187,7 +39983,7 @@
         <v>0</v>
       </c>
       <c r="Q259" s="33" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40240,7 +40036,7 @@
         <v>0</v>
       </c>
       <c r="Q260" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="112.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40293,7 +40089,7 @@
         <v>0</v>
       </c>
       <c r="Q261" s="33" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40346,7 +40142,7 @@
         <v>0</v>
       </c>
       <c r="Q262" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40399,7 +40195,7 @@
         <v>0</v>
       </c>
       <c r="Q263" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40452,7 +40248,7 @@
         <v>0</v>
       </c>
       <c r="Q264" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40505,7 +40301,7 @@
         <v>0</v>
       </c>
       <c r="Q265" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40558,7 +40354,7 @@
         <v>0</v>
       </c>
       <c r="Q266" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40611,7 +40407,7 @@
         <v>0</v>
       </c>
       <c r="Q267" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40664,7 +40460,7 @@
         <v>0</v>
       </c>
       <c r="Q268" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40717,7 +40513,7 @@
         <v>0</v>
       </c>
       <c r="Q269" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40770,7 +40566,7 @@
         <v>0</v>
       </c>
       <c r="Q270" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40823,7 +40619,7 @@
         <v>0</v>
       </c>
       <c r="Q271" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40876,7 +40672,7 @@
         <v>0</v>
       </c>
       <c r="Q272" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40929,7 +40725,7 @@
         <v>0</v>
       </c>
       <c r="Q273" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40982,7 +40778,7 @@
         <v>0</v>
       </c>
       <c r="Q274" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41035,7 +40831,7 @@
         <v>0</v>
       </c>
       <c r="Q275" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41088,7 +40884,7 @@
         <v>0</v>
       </c>
       <c r="Q276" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41141,7 +40937,7 @@
         <v>0</v>
       </c>
       <c r="Q277" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41194,7 +40990,7 @@
         <v>0</v>
       </c>
       <c r="Q278" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41247,7 +41043,7 @@
         <v>0</v>
       </c>
       <c r="Q279" s="33" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41300,7 +41096,7 @@
         <v>0</v>
       </c>
       <c r="Q280" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41353,7 +41149,7 @@
         <v>0</v>
       </c>
       <c r="Q281" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41406,7 +41202,7 @@
         <v>0</v>
       </c>
       <c r="Q282" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41459,7 +41255,7 @@
         <v>0</v>
       </c>
       <c r="Q283" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41512,7 +41308,7 @@
         <v>0</v>
       </c>
       <c r="Q284" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41565,7 +41361,7 @@
         <v>0</v>
       </c>
       <c r="Q285" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41618,7 +41414,7 @@
         <v>0</v>
       </c>
       <c r="Q286" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41671,7 +41467,7 @@
         <v>0</v>
       </c>
       <c r="Q287" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41724,7 +41520,7 @@
         <v>0</v>
       </c>
       <c r="Q288" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41777,7 +41573,7 @@
         <v>0</v>
       </c>
       <c r="Q289" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41830,7 +41626,7 @@
         <v>0</v>
       </c>
       <c r="Q290" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41883,7 +41679,7 @@
         <v>0</v>
       </c>
       <c r="Q291" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41936,7 +41732,7 @@
         <v>0</v>
       </c>
       <c r="Q292" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41989,7 +41785,7 @@
         <v>0</v>
       </c>
       <c r="Q293" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42042,7 +41838,7 @@
         <v>0</v>
       </c>
       <c r="Q294" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42095,7 +41891,7 @@
         <v>0</v>
       </c>
       <c r="Q295" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42148,7 +41944,7 @@
         <v>0</v>
       </c>
       <c r="Q296" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42201,7 +41997,7 @@
         <v>0</v>
       </c>
       <c r="Q297" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42254,7 +42050,7 @@
         <v>0</v>
       </c>
       <c r="Q298" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42307,7 +42103,7 @@
         <v>0</v>
       </c>
       <c r="Q299" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42360,7 +42156,7 @@
         <v>0</v>
       </c>
       <c r="Q300" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42413,7 +42209,7 @@
         <v>0</v>
       </c>
       <c r="Q301" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42466,7 +42262,7 @@
         <v>0</v>
       </c>
       <c r="Q302" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42519,7 +42315,7 @@
         <v>0</v>
       </c>
       <c r="Q303" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42572,7 +42368,7 @@
         <v>0</v>
       </c>
       <c r="Q304" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42625,7 +42421,7 @@
         <v>0</v>
       </c>
       <c r="Q305" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42678,7 +42474,7 @@
         <v>0</v>
       </c>
       <c r="Q306" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42731,7 +42527,7 @@
         <v>0</v>
       </c>
       <c r="Q307" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42784,7 +42580,7 @@
         <v>0</v>
       </c>
       <c r="Q308" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42837,7 +42633,7 @@
         <v>0</v>
       </c>
       <c r="Q309" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42890,7 +42686,7 @@
         <v>0</v>
       </c>
       <c r="Q310" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42943,7 +42739,7 @@
         <v>0</v>
       </c>
       <c r="Q311" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42996,7 +42792,7 @@
         <v>0</v>
       </c>
       <c r="Q312" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43049,7 +42845,7 @@
         <v>0</v>
       </c>
       <c r="Q313" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43102,7 +42898,7 @@
         <v>0</v>
       </c>
       <c r="Q314" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43155,7 +42951,7 @@
         <v>0</v>
       </c>
       <c r="Q315" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43208,7 +43004,7 @@
         <v>0</v>
       </c>
       <c r="Q316" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43261,7 +43057,7 @@
         <v>0</v>
       </c>
       <c r="Q317" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43314,7 +43110,7 @@
         <v>0</v>
       </c>
       <c r="Q318" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43367,7 +43163,7 @@
         <v>0</v>
       </c>
       <c r="Q319" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43420,7 +43216,7 @@
         <v>0</v>
       </c>
       <c r="Q320" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43473,7 +43269,7 @@
         <v>0</v>
       </c>
       <c r="Q321" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43526,7 +43322,7 @@
         <v>0</v>
       </c>
       <c r="Q322" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43579,7 +43375,7 @@
         <v>0</v>
       </c>
       <c r="Q323" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43632,7 +43428,7 @@
         <v>0</v>
       </c>
       <c r="Q324" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43685,7 +43481,7 @@
         <v>0</v>
       </c>
       <c r="Q325" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43738,7 +43534,7 @@
         <v>0</v>
       </c>
       <c r="Q326" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43791,7 +43587,7 @@
         <v>0</v>
       </c>
       <c r="Q327" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43844,7 +43640,7 @@
         <v>0</v>
       </c>
       <c r="Q328" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43897,7 +43693,7 @@
         <v>0</v>
       </c>
       <c r="Q329" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43950,7 +43746,7 @@
         <v>0</v>
       </c>
       <c r="Q330" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44003,7 +43799,7 @@
         <v>0</v>
       </c>
       <c r="Q331" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44056,7 +43852,7 @@
         <v>0</v>
       </c>
       <c r="Q332" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44109,7 +43905,7 @@
         <v>0</v>
       </c>
       <c r="Q333" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44162,7 +43958,7 @@
         <v>0</v>
       </c>
       <c r="Q334" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44215,7 +44011,7 @@
         <v>0</v>
       </c>
       <c r="Q335" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44268,7 +44064,7 @@
         <v>0</v>
       </c>
       <c r="Q336" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44321,7 +44117,7 @@
         <v>0</v>
       </c>
       <c r="Q337" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44374,7 +44170,7 @@
         <v>0</v>
       </c>
       <c r="Q338" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44427,7 +44223,7 @@
         <v>0</v>
       </c>
       <c r="Q339" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44480,7 +44276,7 @@
         <v>0</v>
       </c>
       <c r="Q340" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44533,7 +44329,7 @@
         <v>0</v>
       </c>
       <c r="Q341" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44586,7 +44382,7 @@
         <v>0</v>
       </c>
       <c r="Q342" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44639,7 +44435,7 @@
         <v>0</v>
       </c>
       <c r="Q343" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44692,7 +44488,7 @@
         <v>0</v>
       </c>
       <c r="Q344" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44745,7 +44541,7 @@
         <v>0</v>
       </c>
       <c r="Q345" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44798,7 +44594,7 @@
         <v>0</v>
       </c>
       <c r="Q346" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44851,7 +44647,7 @@
         <v>0</v>
       </c>
       <c r="Q347" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44904,7 +44700,7 @@
         <v>0</v>
       </c>
       <c r="Q348" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44957,7 +44753,7 @@
         <v>0</v>
       </c>
       <c r="Q349" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45010,7 +44806,7 @@
         <v>0</v>
       </c>
       <c r="Q350" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45063,7 +44859,7 @@
         <v>0</v>
       </c>
       <c r="Q351" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45116,7 +44912,7 @@
         <v>0</v>
       </c>
       <c r="Q352" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45169,7 +44965,7 @@
         <v>0</v>
       </c>
       <c r="Q353" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45222,7 +45018,7 @@
         <v>0</v>
       </c>
       <c r="Q354" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45275,7 +45071,7 @@
         <v>0</v>
       </c>
       <c r="Q355" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45328,7 +45124,7 @@
         <v>0</v>
       </c>
       <c r="Q356" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45381,7 +45177,7 @@
         <v>0</v>
       </c>
       <c r="Q357" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45434,7 +45230,7 @@
         <v>0</v>
       </c>
       <c r="Q358" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45487,7 +45283,7 @@
         <v>0</v>
       </c>
       <c r="Q359" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45540,7 +45336,7 @@
         <v>0</v>
       </c>
       <c r="Q360" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45593,7 +45389,7 @@
         <v>0</v>
       </c>
       <c r="Q361" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45646,7 +45442,7 @@
         <v>0</v>
       </c>
       <c r="Q362" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45699,7 +45495,7 @@
         <v>0</v>
       </c>
       <c r="Q363" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45752,7 +45548,7 @@
         <v>0</v>
       </c>
       <c r="Q364" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45805,7 +45601,7 @@
         <v>0</v>
       </c>
       <c r="Q365" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>